<commit_message>
reglas _ largo del argumento
largo del argumento definido en reglas
largo implementado en “debate” argumento
en argumento muestra la cantidad de caracteres restantes
</commit_message>
<xml_diff>
--- a/Documentación/Sprints/AnalisisDiseño_Sprint1-6.xlsx
+++ b/Documentación/Sprints/AnalisisDiseño_Sprint1-6.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Paula/ICI 2013/VIII Semestre/Taller Ing Software/RedDebate/Documentación/Sprints/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Daniel/Documents/project/RedDebate/Documentación/Sprints/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Análisis1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,6 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>El sistema enviará un mensaje de error indicando que es necesario un argumento inicial al debate. El sistema no cargará los datos a la base de datos y no recargará la página.</t>
   </si>
@@ -80,6 +77,126 @@
   </si>
   <si>
     <t>Precondicion</t>
+  </si>
+  <si>
+    <t>Resumen</t>
+  </si>
+  <si>
+    <t>iniciar, definir y publicar debate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposito </t>
+  </si>
+  <si>
+    <t>Creador, participante</t>
+  </si>
+  <si>
+    <t>Actores</t>
+  </si>
+  <si>
+    <t>Crear debate</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPRINT 1 </t>
+  </si>
+  <si>
+    <t>postcondiciones</t>
+  </si>
+  <si>
+    <t>precondiciones</t>
+  </si>
+  <si>
+    <t>salida</t>
+  </si>
+  <si>
+    <t>excepciones</t>
+  </si>
+  <si>
+    <t>notas</t>
+  </si>
+  <si>
+    <t>Sistema</t>
+  </si>
+  <si>
+    <t>responsabilidades</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>El sistema conoce el id del usuario</t>
+  </si>
+  <si>
+    <t>Si el id del usuario no es valido, indicar error</t>
+  </si>
+  <si>
+    <t>usuario tenga una cuenta en Facebook</t>
+  </si>
+  <si>
+    <t>ingreso()</t>
+  </si>
+  <si>
+    <t>Contratos</t>
+  </si>
+  <si>
+    <t>(1) Se creó instancia usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caso de uso </t>
+  </si>
+  <si>
+    <t>Diagrama de Secuencia</t>
+  </si>
+  <si>
+    <t>Permitir que un usuario ingresar a la aplicación a través de un login.
+Solicitar el despliegue del formulario de creación de debate</t>
+  </si>
+  <si>
+    <t>(1) Se creó instancia debate
+(2) Se agrega el debate al almacen de debates</t>
+  </si>
+  <si>
+    <t>el sistema conoce el id del debate</t>
+  </si>
+  <si>
+    <t>pubicar_debate()</t>
+  </si>
+  <si>
+    <t>inscribir_debate(titulo,arg,fecha)</t>
+  </si>
+  <si>
+    <t>solicitar_depliegue()</t>
+  </si>
+  <si>
+    <t>desplegar todos los debates en la página principal</t>
+  </si>
+  <si>
+    <t>(1) se buscaron todos los debates con estado público
+(2) se entregó el listado de los debates públicos</t>
+  </si>
+  <si>
+    <t>Modelo Conceptual</t>
+  </si>
+  <si>
+    <t>Diagrama de estados</t>
+  </si>
+  <si>
+    <t>Diagrama de Colaboración</t>
+  </si>
+  <si>
+    <t>Debate: se agrega el atributo "limite " y fecha limite y alias_usuario = False</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Usuario = nuevo atributo "Alias = anonimo x defecto"</t>
+  </si>
+  <si>
+    <t>5. El usuario ingresa un título del debate y su argumento inicial en los campos respectivos del formulario desplegado, opcionalmente incluye un largo máximo por argumento (máximo por defecto: 300 caracteres), la fecha de finalización del debate(por defecto indefinido) y si quiere usar su nombre "alias" (no por defecto) , para finalizar oprime "publicar".</t>
   </si>
   <si>
     <r>
@@ -100,129 +217,36 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve"> llega al inicio del sistema y oprime el botón 'crear debate' donde se despliega un formulario de creación de debate, con los campos 'título' y 'argumento inicial'. Luego de llenar los campos el creador oprime 'Publicar'. El debate estará desplegado en la ventana inicio disponible para que un usuario participante interactúe con el</t>
+      <t xml:space="preserve"> llega al inicio del sistema y oprime el botón 'crear debate' donde se despliega un formulario de creación de debate, con los campos 'título' y 'argumento inicial' y la sección reglas con los campos: largo máximo argumento, fecha de finalización del debate y alias (usuario muestra su nombre como creado o no). Luego de llenar los campos el creador oprime 'Publicar'. El debate estará desplegado en la ventana inicio disponible para que un usuario participante interactúe con el</t>
     </r>
   </si>
   <si>
-    <t>Resumen</t>
-  </si>
-  <si>
-    <t>iniciar, definir y publicar debate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposito </t>
-  </si>
-  <si>
-    <t>Creador, participante</t>
-  </si>
-  <si>
-    <t>Actores</t>
-  </si>
-  <si>
-    <t>Crear debate</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPRINT 1 </t>
-  </si>
-  <si>
-    <t>postcondiciones</t>
-  </si>
-  <si>
-    <t>precondiciones</t>
-  </si>
-  <si>
-    <t>salida</t>
-  </si>
-  <si>
-    <t>excepciones</t>
-  </si>
-  <si>
-    <t>notas</t>
-  </si>
-  <si>
-    <t>Sistema</t>
-  </si>
-  <si>
-    <t>responsabilidades</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>El sistema conoce el id del usuario</t>
-  </si>
-  <si>
-    <t>Si el id del usuario no es valido, indicar error</t>
-  </si>
-  <si>
-    <t>usuario tenga una cuenta en Facebook</t>
-  </si>
-  <si>
-    <t>ingreso()</t>
-  </si>
-  <si>
-    <t>Contratos</t>
-  </si>
-  <si>
-    <t>(1) Se creó instancia usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caso de uso </t>
-  </si>
-  <si>
-    <t>Diagrama de Secuencia</t>
-  </si>
-  <si>
-    <t>Permitir que un usuario ingresar a la aplicación a través de un login.
-Solicitar el despliegue del formulario de creación de debate</t>
-  </si>
-  <si>
-    <t>Capturar el usuario, titulo del debate, la descripcion inicial y la fecha para agregarla a un nuevo debate</t>
-  </si>
-  <si>
-    <t>(1) Se creó instancia debate
-(2) Se agrega el debate al almacen de debates</t>
-  </si>
-  <si>
-    <t>el sistema conoce el id del debate</t>
-  </si>
-  <si>
-    <t>pubicar_debate()</t>
-  </si>
-  <si>
-    <t>inscribir_debate(titulo,arg,fecha)</t>
-  </si>
-  <si>
-    <t>actualizar el estado del debate a público</t>
+    <t>5. El usuario ingresa un número superior a 300 en el largo máximo de caracteres en argumento</t>
+  </si>
+  <si>
+    <t>El sistema enviará un mensaje de error indicando que se superó el número máximo de caracteres en el argumento. El sistema no cargará los datos a la base de datos y no recargará la página.</t>
+  </si>
+  <si>
+    <t>Capturar el usuario, titulo del debate, la descripcion inicial y la fecha para agregarla a un nuevo debate
+Capturar el largo , fecha de finalizacion, alias_creador en caso de no ser la configuración por defecto</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>D= crear_debate(U,titulo, arg, fecha, largo,fecha_fin, alias_c )</t>
+  </si>
+  <si>
+    <t>actualizar el estado del debate a público
+cerrar el debate en caso de haber pasado la fecha de finalizacion</t>
   </si>
   <si>
     <t>(1) se buscó el debate en el almacen de debates
-(2) se modificó el estado del debate a público</t>
-  </si>
-  <si>
-    <t>solicitar_depliegue()</t>
-  </si>
-  <si>
-    <t>desplegar todos los debates en la página principal</t>
-  </si>
-  <si>
-    <t>(1) se buscaron todos los debates con estado público
-(2) se entregó el listado de los debates públicos</t>
-  </si>
-  <si>
-    <t>5. El usuario ingresa un título del debate y su argumento inicial en los campos respectivos del formulario desplegado , para finalizar oprime "publicar".</t>
-  </si>
-  <si>
-    <t>Modelo Conceptual</t>
-  </si>
-  <si>
-    <t>Diagrama de estados</t>
-  </si>
-  <si>
-    <t>Diagrama de Colaboración</t>
+(2) se modificó el estado del debate a público
+(3) si el debate está abierto, y si la fecha_fin ya pasó, entonces se cerró el debate</t>
+  </si>
+  <si>
+    <t>3: actualizar_cierre(B)</t>
   </si>
 </sst>
 </file>
@@ -533,91 +557,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,19 +661,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>29306</xdr:colOff>
+      <xdr:colOff>9769</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>38541</xdr:rowOff>
+      <xdr:rowOff>39077</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>410308</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>922197</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>803030</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>266826</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -662,8 +686,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7619998" y="1181541"/>
-          <a:ext cx="5363310" cy="1469810"/>
+          <a:off x="7600461" y="1182077"/>
+          <a:ext cx="7915031" cy="3412518"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -687,8 +711,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>224366</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -725,8 +749,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>322116</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>5773</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>605213</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1112,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F20"/>
+  <dimension ref="B1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="C8" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1126,169 +1150,198 @@
     <col min="4" max="4" width="48.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="17.1640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="2:6" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="2:6" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="F3" s="38" t="s">
+    <row r="1" spans="2:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="2:11" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="17"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="2:11" ht="91" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="F3" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="25" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="26"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="15" t="s">
+      <c r="C4" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="D4" s="35"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="27"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="15" t="s">
+      <c r="C5" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="D5" s="36"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="27"/>
-    </row>
-    <row r="7" spans="2:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="15" t="s">
+      <c r="C6" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="D6" s="36"/>
+    </row>
+    <row r="7" spans="2:11" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="27"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="15" t="s">
+      <c r="C7" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="36"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="27"/>
-    </row>
-    <row r="9" spans="2:6" ht="21" x14ac:dyDescent="0.2">
-      <c r="B9" s="15" t="s">
+      <c r="C8" s="34"/>
+      <c r="D8" s="36"/>
+    </row>
+    <row r="9" spans="2:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="B9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="F9" s="38"/>
-    </row>
-    <row r="10" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="D9" s="36"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="2:6" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
+    </row>
+    <row r="11" spans="2:11" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="35" t="s">
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="37" t="s">
+      <c r="C13" s="32"/>
+      <c r="D13" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="29" t="s">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="30" t="s">
+      <c r="C14" s="34"/>
+      <c r="D14" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="B15" s="29" t="s">
+    <row r="15" spans="2:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="B15" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="30" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="92" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33" t="s">
+    <row r="16" spans="2:11" ht="92" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
     </row>
     <row r="18" spans="2:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="26"/>
     </row>
     <row r="19" spans="2:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="14" t="s">
+      <c r="C19" s="28"/>
+      <c r="D19" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="46" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="17" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="16" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="2:4" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
@@ -1297,14 +1350,6 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1315,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K45"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="156" zoomScalePageLayoutView="156" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A29" zoomScale="125" zoomScaleNormal="156" zoomScalePageLayoutView="156" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1328,44 +1373,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="B1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="B2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="E2" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="38"/>
+      <c r="B2" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="E2" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
@@ -1373,7 +1418,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
@@ -1384,53 +1429,53 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="60" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -1438,7 +1483,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -1449,60 +1494,60 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="6"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="6"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="E24" s="38" t="s">
-        <v>55</v>
+      <c r="E24" s="22" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="30" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
@@ -1510,7 +1555,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
@@ -1521,53 +1566,53 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="6"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="6"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" s="6"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.2">
@@ -1584,34 +1629,34 @@
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C41" s="6"/>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C42" s="6"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C43" s="6"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C44" s="6"/>
     </row>
     <row r="45" spans="2:3" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1625,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B3"/>
+  <dimension ref="B1:O38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1637,13 +1682,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="B1" s="18" t="s">
-        <v>25</v>
+      <c r="B1" s="17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="39" t="s">
-        <v>56</v>
+      <c r="B3" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="14:15" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>60</v>
+      </c>
+      <c r="O19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O38" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>